<commit_message>
Plein de modif mdrr
</commit_message>
<xml_diff>
--- a/NDF/data.xlsx
+++ b/NDF/data.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kilianpouderoux/Documents/Forum/NDF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4627FFC-41D4-9C4C-8004-8E839C81A792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BF8870-E424-9A4C-83A3-9C0FA578C0E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="1000" windowWidth="27640" windowHeight="15360" xr2:uid="{C827883D-5563-CD46-AEBF-421568CE900D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -75,16 +75,66 @@
   </si>
   <si>
     <t>yeahyo</t>
+  </si>
+  <si>
+    <t>Remarque</t>
+  </si>
+  <si>
+    <t>mamma mia</t>
+  </si>
+  <si>
+    <t>zobi</t>
+  </si>
+  <si>
+    <t>OUI</t>
+  </si>
+  <si>
+    <t>NON</t>
+  </si>
+  <si>
+    <t>Générer</t>
+  </si>
+  <si>
+    <t>fst puta</t>
+  </si>
+  <si>
+    <t>ffof</t>
+  </si>
+  <si>
+    <t>qqwfgq</t>
+  </si>
+  <si>
+    <t>fqwef</t>
+  </si>
+  <si>
+    <t>okay</t>
+  </si>
+  <si>
+    <t>que pasa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,9 +160,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,38 +478,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD3406B-009B-0740-9969-94344BD20D4E}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>45284</v>
       </c>
@@ -480,8 +538,14 @@
       <c r="G2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>41255</v>
       </c>
@@ -503,8 +567,392 @@
       <c r="G3" t="s">
         <v>11</v>
       </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>45284</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>45284</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>45284</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>45285</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>45286</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>45287</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>45288</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>45289</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>45290</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>45291</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>45292</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>45293</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>45294</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>